<commit_message>
Add BasePage, BaseClass, logging setup, and log4j2 config
</commit_message>
<xml_diff>
--- a/test-data/testdata_cdcalculator.xlsx
+++ b/test-data/testdata_cdcalculator.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="34">
   <si>
     <t>InitialDeposit</t>
   </si>
@@ -200,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="370">
+  <cellXfs count="418">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -535,6 +535,54 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -960,7 +1008,7 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="346" t="s">
+      <c r="G2" s="394" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="9" t="s">
@@ -986,7 +1034,7 @@
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="347" t="s">
+      <c r="G3" s="395" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -1012,7 +1060,7 @@
       <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="348" t="s">
+      <c r="G4" s="396" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="9" t="s">
@@ -1038,7 +1086,7 @@
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="349" t="s">
+      <c r="G5" s="397" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="9" t="s">
@@ -1064,7 +1112,7 @@
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="350" t="s">
+      <c r="G6" s="398" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -1090,7 +1138,7 @@
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="351" t="s">
+      <c r="G7" s="399" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -1116,7 +1164,7 @@
       <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="352" t="s">
+      <c r="G8" s="400" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -1142,7 +1190,7 @@
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="353" t="s">
+      <c r="G9" s="401" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -1168,7 +1216,7 @@
       <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="354" t="s">
+      <c r="G10" s="402" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -1194,7 +1242,7 @@
       <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="355" t="s">
+      <c r="G11" s="403" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -1220,7 +1268,7 @@
       <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="356" t="s">
+      <c r="G12" s="404" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -1246,7 +1294,7 @@
       <c r="F13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="357" t="s">
+      <c r="G13" s="405" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="9" t="s">
@@ -1327,7 +1375,7 @@
       <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="358" t="s">
+      <c r="H2" s="406" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1353,7 +1401,7 @@
       <c r="G3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="359" t="s">
+      <c r="H3" s="407" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1379,7 +1427,7 @@
       <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="360" t="s">
+      <c r="H4" s="408" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1405,7 +1453,7 @@
       <c r="G5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="361" t="s">
+      <c r="H5" s="409" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1431,7 +1479,7 @@
       <c r="G6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="362" t="s">
+      <c r="H6" s="410" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1457,7 +1505,7 @@
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="363" t="s">
+      <c r="H7" s="411" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1483,7 +1531,7 @@
       <c r="G8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="364" t="s">
+      <c r="H8" s="412" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1509,7 +1557,7 @@
       <c r="G9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="365" t="s">
+      <c r="H9" s="413" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1535,7 +1583,7 @@
       <c r="G10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="366" t="s">
+      <c r="H10" s="414" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1561,7 +1609,7 @@
       <c r="G11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="367" t="s">
+      <c r="H11" s="415" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1587,7 +1635,7 @@
       <c r="G12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="368" t="s">
+      <c r="H12" s="416" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1613,7 +1661,7 @@
       <c r="G13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="369" t="s">
+      <c r="H13" s="417" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add crossbrowsertesting.xml and update testng.xml to master.xml
</commit_message>
<xml_diff>
--- a/test-data/testdata_cdcalculator.xlsx
+++ b/test-data/testdata_cdcalculator.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="34">
   <si>
     <t>InitialDeposit</t>
   </si>
@@ -200,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="418">
+  <cellXfs count="442">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -535,6 +535,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -1008,7 +1032,7 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="394" t="s">
+      <c r="G2" s="418" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="9" t="s">
@@ -1034,7 +1058,7 @@
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="395" t="s">
+      <c r="G3" s="419" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -1060,7 +1084,7 @@
       <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="396" t="s">
+      <c r="G4" s="420" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="9" t="s">
@@ -1086,7 +1110,7 @@
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="397" t="s">
+      <c r="G5" s="421" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="9" t="s">
@@ -1112,7 +1136,7 @@
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="398" t="s">
+      <c r="G6" s="422" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -1138,7 +1162,7 @@
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="399" t="s">
+      <c r="G7" s="423" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -1164,7 +1188,7 @@
       <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="400" t="s">
+      <c r="G8" s="424" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -1190,7 +1214,7 @@
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="401" t="s">
+      <c r="G9" s="425" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -1216,7 +1240,7 @@
       <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="402" t="s">
+      <c r="G10" s="426" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -1242,7 +1266,7 @@
       <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="403" t="s">
+      <c r="G11" s="427" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -1268,7 +1292,7 @@
       <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="404" t="s">
+      <c r="G12" s="428" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -1294,7 +1318,7 @@
       <c r="F13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="405" t="s">
+      <c r="G13" s="429" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="9" t="s">
@@ -1375,7 +1399,7 @@
       <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="406" t="s">
+      <c r="H2" s="430" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1401,7 +1425,7 @@
       <c r="G3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="407" t="s">
+      <c r="H3" s="431" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1427,7 +1451,7 @@
       <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="408" t="s">
+      <c r="H4" s="432" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1453,7 +1477,7 @@
       <c r="G5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="409" t="s">
+      <c r="H5" s="433" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1479,7 +1503,7 @@
       <c r="G6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="410" t="s">
+      <c r="H6" s="434" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1505,7 +1529,7 @@
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="411" t="s">
+      <c r="H7" s="435" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1531,7 +1555,7 @@
       <c r="G8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="412" t="s">
+      <c r="H8" s="436" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1557,7 +1581,7 @@
       <c r="G9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="413" t="s">
+      <c r="H9" s="437" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1583,7 +1607,7 @@
       <c r="G10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="414" t="s">
+      <c r="H10" s="438" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1609,7 +1633,7 @@
       <c r="G11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="415" t="s">
+      <c r="H11" s="439" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1635,7 +1659,7 @@
       <c r="G12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="416" t="s">
+      <c r="H12" s="440" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1661,7 +1685,7 @@
       <c r="G13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="417" t="s">
+      <c r="H13" s="441" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rearranges Test Cases and implement DDT using TestNG Dataproviders
</commit_message>
<xml_diff>
--- a/test-data/testdata_cdcalculator.xlsx
+++ b/test-data/testdata_cdcalculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Automation\automate-citbank-cd-calculator\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Automation\automate-citbank-cd-calculator\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06406810-1DA1-4420-85AD-E9D18F8B0FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553A3A24-A900-48C8-A436-32CC10AC06E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7069F9CF-838F-47F3-875D-916362C89D4D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{7069F9CF-838F-47F3-875D-916362C89D4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Compounded_Daily" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="34">
   <si>
     <t>InitialDeposit</t>
   </si>
@@ -118,16 +118,16 @@
     <t>Status Chrome</t>
   </si>
   <si>
-    <t>Status edge</t>
-  </si>
-  <si>
     <t>Status chrome</t>
   </si>
   <si>
     <t>Status firefox</t>
   </si>
   <si>
-    <t>Failed</t>
+    <t>RowCount</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -200,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="442">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -223,6 +223,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -232,426 +233,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
@@ -971,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4669D5-9AD2-473B-A8EA-5D8F530CC8C4}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1007,10 +588,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1032,7 +613,7 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="418" t="s">
+      <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="9" t="s">
@@ -1058,7 +639,7 @@
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="419" t="s">
+      <c r="G3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -1084,7 +665,7 @@
       <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="420" t="s">
+      <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="9" t="s">
@@ -1110,7 +691,7 @@
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="421" t="s">
+      <c r="G5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="9" t="s">
@@ -1136,7 +717,7 @@
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="422" t="s">
+      <c r="G6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -1162,7 +743,7 @@
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="423" t="s">
+      <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -1188,7 +769,7 @@
       <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="424" t="s">
+      <c r="G8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -1214,7 +795,7 @@
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="425" t="s">
+      <c r="G9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="9" t="s">
@@ -1240,7 +821,7 @@
       <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="426" t="s">
+      <c r="G10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -1266,7 +847,7 @@
       <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="427" t="s">
+      <c r="G11" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -1292,7 +873,7 @@
       <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="428" t="s">
+      <c r="G12" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -1318,7 +899,7 @@
       <c r="F13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="429" t="s">
+      <c r="G13" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="9" t="s">
@@ -1335,357 +916,357 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CE2FBF-79F0-461C-8A13-1762CE45C5DB}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.90625"/>
-    <col min="2" max="2" customWidth="true" width="15.453125"/>
-    <col min="3" max="3" customWidth="true" width="18.6328125"/>
-    <col min="4" max="4" customWidth="true" width="24.08984375"/>
-    <col min="5" max="5" customWidth="true" width="17.0"/>
-    <col min="6" max="6" customWidth="true" width="17.6328125"/>
-    <col min="7" max="7" customWidth="true" width="14.81640625"/>
-    <col min="8" max="8" customWidth="true" width="13.81640625"/>
+    <col min="1" max="1" customWidth="true" width="10.7265625"/>
+    <col min="2" max="2" customWidth="true" width="14.90625"/>
+    <col min="3" max="3" customWidth="true" width="15.453125"/>
+    <col min="4" max="4" customWidth="true" width="18.6328125"/>
+    <col min="5" max="5" customWidth="true" width="24.08984375"/>
+    <col min="6" max="6" customWidth="true" width="17.0"/>
+    <col min="7" max="7" customWidth="true" width="17.6328125"/>
+    <col min="8" max="8" customWidth="true" width="14.81640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>31500</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>13</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="7">
-        <v>32050.75</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="7">
+        <v>32050.39</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="430" t="s">
-        <v>33</v>
+      <c r="H2" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
         <v>50000</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>12</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="7">
-        <v>51010.04</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="7">
+        <v>51009.22</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="431" t="s">
-        <v>33</v>
+      <c r="H3" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
         <v>25000</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1">
         <v>24</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="7">
-        <v>25916.37</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="7">
+        <v>25915.7</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="432" t="s">
-        <v>33</v>
+      <c r="H4" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
         <v>100000</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>60</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="7">
-        <v>113314.36</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="7">
+        <v>113300.11</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="433" t="s">
-        <v>33</v>
+      <c r="H5" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
         <v>15000</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="1">
         <v>36</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="7">
-        <v>15643.4</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="7">
+        <v>15643.03</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="434" t="s">
-        <v>33</v>
+      <c r="H6" s="15" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>1</v>
+      <c r="A7" s="0">
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="7">
+      <c r="F7" s="7">
         <v>1</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="435" t="s">
+      <c r="H7" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
         <v>9999999</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="1">
         <v>120</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="7">
-        <v>16486646.49</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="7">
+        <v>16470093.33</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="436" t="s">
+      <c r="H8" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>30000</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="7">
+        <v>31981.41</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="0">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>30000</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-12</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="7">
+        <v>30483.54</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>30000</v>
+      </c>
+      <c r="C11" s="1">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="7">
+        <v>30483.85</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
         <v>30000</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C12" s="1">
+        <v>12</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="7">
+        <v>30301.5</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="0">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
         <v>0</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C13" s="1">
+        <v>12</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="7">
-        <v>16486646.49</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="437" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>30000</v>
-      </c>
-      <c r="B10" s="1">
-        <v>-12</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="7">
-        <v>30483.85</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="438" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>30000</v>
-      </c>
-      <c r="B11" s="1">
-        <v>12</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="7">
-        <v>30483.85</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="439" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>30000</v>
-      </c>
-      <c r="B12" s="1">
-        <v>12</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="7">
+      <c r="F13" s="7">
         <v>30301.5</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="440" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1">
-        <v>12</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="7">
-        <v>30301.5</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="441" t="s">
+      <c r="H13" s="22" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added more test cases with restructing framework, adding grouping.xml to run sanity,smoke and regreesion test cases
</commit_message>
<xml_diff>
--- a/test-data/testdata_cdcalculator.xlsx
+++ b/test-data/testdata_cdcalculator.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="34">
   <si>
     <t>InitialDeposit</t>
   </si>
@@ -200,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -224,6 +224,43 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -980,7 +1017,7 @@
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="48" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1006,7 +1043,7 @@
       <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="49" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1032,7 +1069,7 @@
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="50" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1058,7 +1095,7 @@
       <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="51" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1084,7 +1121,7 @@
       <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="52" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1110,7 +1147,7 @@
       <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="53" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1136,7 +1173,7 @@
       <c r="G8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="54" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1162,7 +1199,7 @@
       <c r="G9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="55" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1188,7 +1225,7 @@
       <c r="G10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="56" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1214,7 +1251,7 @@
       <c r="G11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="57" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1240,7 +1277,7 @@
       <c r="G12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="58" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1266,7 +1303,7 @@
       <c r="G13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="59" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>